<commit_message>
Added unit tests for sorting algorithms and statistics. Need to complete the spread stats unit tests
</commit_message>
<xml_diff>
--- a/Documentation/Q5031372-ArtifactDiary/Product & Sprint Backlog.xlsx
+++ b/Documentation/Q5031372-ArtifactDiary/Product & Sprint Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Year Three\ComputingProject\ShellTemperature\Documentation\Q5031372-ArtifactDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749C4F95-2480-4078-8924-2C7932B2A0EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003F7407-C5E8-4464-83C8-5EE207F07BD2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46305" yWindow="6360" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Sprint Four" sheetId="7" r:id="rId5"/>
     <sheet name="Sprint Five" sheetId="8" r:id="rId6"/>
     <sheet name="Sprint Six" sheetId="9" r:id="rId7"/>
+    <sheet name="Sprint Seven" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="181">
   <si>
     <t>UserStoryID</t>
   </si>
@@ -577,6 +578,9 @@
   <si>
     <t>Retrieve the temperature values between a date range and calculate all data statistics and output to the user</t>
   </si>
+  <si>
+    <t>02/03/2020 - 08/03/2020</t>
+  </si>
 </sst>
 </file>
 
@@ -1097,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1472,12 +1476,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1519,6 +1517,16 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4687,6 +4695,610 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Points Remaining each day and Average points remaining</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint Seven'!$O$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Points Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint Seven'!$M$13:$M$19</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sat</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sun</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Seven'!$O$13:$O$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B989-4CFC-9660-E75C9972AD6E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint Seven'!$P$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average points remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint Seven'!$M$13:$M$19</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sat</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sun</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Seven'!$P$13:$P$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>102.85714285714286</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85.714285714285722</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68.571428571428584</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.428571428571445</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.285714285714306</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.142857142857164</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B989-4CFC-9660-E75C9972AD6E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="344594824"/>
+        <c:axId val="344591544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="344594824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Day of Week</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="344591544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="344591544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Points</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="344594824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4808,6 +5420,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6911,6 +7563,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
@@ -7131,6 +8299,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE8EFA7E-B94D-429F-9252-7478D2DD0196}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>257174</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0589BC68-FB78-45FD-8374-41B942913004}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7398,10 +8609,10 @@
       <c r="G1" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="148" t="s">
+      <c r="I1" s="146" t="s">
         <v>157</v>
       </c>
-      <c r="J1" s="148" t="s">
+      <c r="J1" s="146" t="s">
         <v>158</v>
       </c>
     </row>
@@ -7427,11 +8638,11 @@
       <c r="G2" s="52">
         <v>43856</v>
       </c>
-      <c r="I2" s="149">
+      <c r="I2" s="147">
         <f>SUM(C2:C24)</f>
         <v>772</v>
       </c>
-      <c r="J2" s="149">
+      <c r="J2" s="147">
         <f>I2 / 12</f>
         <v>64.333333333333329</v>
       </c>
@@ -11883,8 +13094,8 @@
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11922,28 +13133,28 @@
       <c r="B5" s="14"/>
     </row>
     <row r="6" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="136" t="s">
+      <c r="A6" s="153" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="153"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="136"/>
-      <c r="B7" s="136"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
+      <c r="A7" s="153"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="153"/>
     </row>
     <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="134" t="s">
+      <c r="A11" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="152"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
@@ -12030,7 +13241,7 @@
         <v>29</v>
       </c>
       <c r="N13" s="98">
-        <f>D30</f>
+        <f>D29</f>
         <v>6</v>
       </c>
       <c r="O13" s="100">
@@ -12085,7 +13296,7 @@
         <v>30</v>
       </c>
       <c r="N14" s="98">
-        <f>E30</f>
+        <f>E29</f>
         <v>6</v>
       </c>
       <c r="O14" s="100">
@@ -12133,7 +13344,7 @@
         <v>32</v>
       </c>
       <c r="N15" s="98">
-        <f>F30</f>
+        <f>F29</f>
         <v>29</v>
       </c>
       <c r="O15" s="100">
@@ -12181,7 +13392,7 @@
         <v>33</v>
       </c>
       <c r="N16" s="98">
-        <f>G30</f>
+        <f>G29</f>
         <v>6</v>
       </c>
       <c r="O16" s="100">
@@ -12229,7 +13440,7 @@
         <v>34</v>
       </c>
       <c r="N17" s="98">
-        <f>H30</f>
+        <f>H29</f>
         <v>6</v>
       </c>
       <c r="O17" s="100">
@@ -12277,7 +13488,7 @@
         <v>35</v>
       </c>
       <c r="N18" s="98">
-        <f>I30</f>
+        <f>I29</f>
         <v>0</v>
       </c>
       <c r="O18" s="100">
@@ -12305,7 +13516,7 @@
         <v>36</v>
       </c>
       <c r="N19" s="98">
-        <f>J30</f>
+        <f>J29</f>
         <v>12</v>
       </c>
       <c r="O19" s="100">
@@ -12593,40 +13804,42 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="43" t="s">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="45">
-        <f>SUM(D20,D14)</f>
+      <c r="C29" s="44"/>
+      <c r="D29" s="45">
+        <f t="shared" ref="D29:J29" si="2">SUM(D20,D14)</f>
         <v>6</v>
       </c>
-      <c r="E30" s="45">
-        <f t="shared" ref="E30:J30" si="2">SUM(E20,E14)</f>
+      <c r="E29" s="45">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="F30" s="45">
+      <c r="F29" s="45">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="G30" s="45">
+      <c r="G29" s="45">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H30" s="45">
+      <c r="H29" s="45">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="I30" s="45">
+      <c r="I29" s="45">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J30" s="45">
+      <c r="J29" s="45">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="K30" s="46"/>
+      <c r="K29" s="46"/>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L30" s="105"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12661,8 +13874,8 @@
   </sheetPr>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12701,67 +13914,67 @@
         <v>31</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="G5" s="137" t="s">
+      <c r="G5" s="154" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="137"/>
-      <c r="I5" s="137"/>
-      <c r="J5" s="137"/>
-      <c r="K5" s="137"/>
-      <c r="L5" s="137"/>
-      <c r="M5" s="137"/>
-      <c r="N5" s="137"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="154"/>
+      <c r="L5" s="154"/>
+      <c r="M5" s="154"/>
+      <c r="N5" s="154"/>
     </row>
     <row r="6" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="136" t="s">
+      <c r="A6" s="153" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="G6" s="136" t="s">
+      <c r="B6" s="153"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="153"/>
+      <c r="G6" s="153" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="136"/>
-      <c r="M6" s="136"/>
-      <c r="N6" s="136"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="153"/>
+      <c r="M6" s="153"/>
+      <c r="N6" s="153"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="136"/>
-      <c r="B7" s="136"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="136"/>
-      <c r="I7" s="136"/>
-      <c r="J7" s="136"/>
-      <c r="K7" s="136"/>
-      <c r="L7" s="136"/>
-      <c r="M7" s="136"/>
-      <c r="N7" s="136"/>
+      <c r="A7" s="153"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="153"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="153"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
+      <c r="L7" s="153"/>
+      <c r="M7" s="153"/>
+      <c r="N7" s="153"/>
     </row>
     <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="136"/>
-      <c r="L8" s="136"/>
-      <c r="M8" s="136"/>
-      <c r="N8" s="136"/>
+      <c r="G8" s="153"/>
+      <c r="H8" s="153"/>
+      <c r="I8" s="153"/>
+      <c r="J8" s="153"/>
+      <c r="K8" s="153"/>
+      <c r="L8" s="153"/>
+      <c r="M8" s="153"/>
+      <c r="N8" s="153"/>
     </row>
     <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="134" t="s">
+      <c r="A11" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="152"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
@@ -12839,7 +14052,7 @@
         <v>43862</v>
       </c>
       <c r="J13" s="91">
-        <v>43892</v>
+        <v>43863</v>
       </c>
       <c r="K13" s="26" t="s">
         <v>46</v>
@@ -13348,7 +14561,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="47"/>
       <c r="B26" s="60" t="s">
         <v>66</v>
@@ -13413,7 +14626,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="60" t="s">
         <v>68</v>
       </c>
@@ -13443,7 +14656,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="60" t="s">
         <v>69</v>
       </c>
@@ -13475,7 +14688,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="60" t="s">
         <v>70</v>
       </c>
@@ -13508,7 +14721,7 @@
       </c>
       <c r="L30" s="105"/>
     </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="60" t="s">
         <v>71</v>
       </c>
@@ -14100,10 +15313,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14142,65 +15355,65 @@
         <v>31</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="G5" s="137" t="s">
+      <c r="G5" s="154" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="137"/>
-      <c r="I5" s="137"/>
-      <c r="J5" s="137"/>
-      <c r="K5" s="137"/>
-      <c r="L5" s="137"/>
-      <c r="M5" s="137"/>
-      <c r="N5" s="137"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="154"/>
+      <c r="L5" s="154"/>
+      <c r="M5" s="154"/>
+      <c r="N5" s="154"/>
     </row>
     <row r="6" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="136" t="s">
+      <c r="A6" s="153" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="136"/>
-      <c r="M6" s="136"/>
-      <c r="N6" s="136"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="153"/>
+      <c r="G6" s="153"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="153"/>
+      <c r="M6" s="153"/>
+      <c r="N6" s="153"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="136"/>
-      <c r="B7" s="136"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="136"/>
-      <c r="I7" s="136"/>
-      <c r="J7" s="136"/>
-      <c r="K7" s="136"/>
-      <c r="L7" s="136"/>
-      <c r="M7" s="136"/>
-      <c r="N7" s="136"/>
+      <c r="A7" s="153"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="153"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="153"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
+      <c r="L7" s="153"/>
+      <c r="M7" s="153"/>
+      <c r="N7" s="153"/>
     </row>
     <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="136"/>
-      <c r="L8" s="136"/>
-      <c r="M8" s="136"/>
-      <c r="N8" s="136"/>
+      <c r="G8" s="153"/>
+      <c r="H8" s="153"/>
+      <c r="I8" s="153"/>
+      <c r="J8" s="153"/>
+      <c r="K8" s="153"/>
+      <c r="L8" s="153"/>
+      <c r="M8" s="153"/>
+      <c r="N8" s="153"/>
     </row>
     <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="134" t="s">
+      <c r="A11" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="152"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
@@ -14287,15 +15500,15 @@
         <v>29</v>
       </c>
       <c r="N13" s="98">
-        <f>D39</f>
+        <f>D37</f>
         <v>20</v>
       </c>
       <c r="O13" s="100">
-        <f>C39 - N13</f>
+        <f>C37 - N13</f>
         <v>45</v>
       </c>
       <c r="P13" s="99">
-        <f>C39 - N22</f>
+        <f>C37 - N22</f>
         <v>55.714285714285715</v>
       </c>
     </row>
@@ -14342,7 +15555,7 @@
         <v>30</v>
       </c>
       <c r="N14" s="98">
-        <f>E39</f>
+        <f>E37</f>
         <v>10</v>
       </c>
       <c r="O14" s="100">
@@ -14390,7 +15603,7 @@
         <v>32</v>
       </c>
       <c r="N15" s="98">
-        <f>F39</f>
+        <f>F37</f>
         <v>10</v>
       </c>
       <c r="O15" s="100">
@@ -14438,7 +15651,7 @@
         <v>33</v>
       </c>
       <c r="N16" s="98">
-        <f>G39</f>
+        <f>G37</f>
         <v>2</v>
       </c>
       <c r="O16" s="100">
@@ -14486,7 +15699,7 @@
         <v>34</v>
       </c>
       <c r="N17" s="98">
-        <f>H39</f>
+        <f>H37</f>
         <v>13</v>
       </c>
       <c r="O17" s="100">
@@ -14534,7 +15747,7 @@
         <v>35</v>
       </c>
       <c r="N18" s="98">
-        <f>I39</f>
+        <f>I37</f>
         <v>0</v>
       </c>
       <c r="O18" s="100">
@@ -14582,7 +15795,7 @@
         <v>36</v>
       </c>
       <c r="N19" s="98">
-        <f>J39</f>
+        <f>J37</f>
         <v>0</v>
       </c>
       <c r="O19" s="100">
@@ -14685,7 +15898,7 @@
         <v>84</v>
       </c>
       <c r="N22" s="104">
-        <f xml:space="preserve"> C39 / 7</f>
+        <f xml:space="preserve"> C37 / 7</f>
         <v>9.2857142857142865</v>
       </c>
     </row>
@@ -15102,43 +16315,43 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="43" t="s">
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="111">
-        <f>SUM(C31,C27,C22,C14)</f>
+      <c r="C37" s="111">
+        <f t="shared" ref="C37:J37" si="3">SUM(C31,C27,C22,C14)</f>
         <v>65</v>
       </c>
-      <c r="D39" s="111">
-        <f>SUM(D31,D27,D22,D14)</f>
+      <c r="D37" s="111">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="E39" s="111">
-        <f t="shared" ref="E39:J39" si="3">SUM(E31,E27,E22,E14)</f>
-        <v>10</v>
-      </c>
-      <c r="F39" s="111">
+      <c r="E37" s="111">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="G39" s="111">
+      <c r="F37" s="111">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G37" s="111">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="H39" s="111">
+      <c r="H37" s="111">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="I39" s="111">
+      <c r="I37" s="111">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J39" s="111">
+      <c r="J37" s="111">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K39" s="46"/>
+      <c r="K37" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -15161,8 +16374,8 @@
   </sheetPr>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15201,65 +16414,65 @@
         <v>31</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="G5" s="137" t="s">
+      <c r="G5" s="154" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="137"/>
-      <c r="I5" s="137"/>
-      <c r="J5" s="137"/>
-      <c r="K5" s="137"/>
-      <c r="L5" s="137"/>
-      <c r="M5" s="137"/>
-      <c r="N5" s="137"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="154"/>
+      <c r="L5" s="154"/>
+      <c r="M5" s="154"/>
+      <c r="N5" s="154"/>
     </row>
     <row r="6" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="136" t="s">
+      <c r="A6" s="153" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="136"/>
-      <c r="M6" s="136"/>
-      <c r="N6" s="136"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="153"/>
+      <c r="G6" s="153"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="153"/>
+      <c r="M6" s="153"/>
+      <c r="N6" s="153"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="136"/>
-      <c r="B7" s="136"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="136"/>
-      <c r="I7" s="136"/>
-      <c r="J7" s="136"/>
-      <c r="K7" s="136"/>
-      <c r="L7" s="136"/>
-      <c r="M7" s="136"/>
-      <c r="N7" s="136"/>
+      <c r="A7" s="153"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="153"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="153"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
+      <c r="L7" s="153"/>
+      <c r="M7" s="153"/>
+      <c r="N7" s="153"/>
     </row>
     <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="136"/>
-      <c r="L8" s="136"/>
-      <c r="M8" s="136"/>
-      <c r="N8" s="136"/>
+      <c r="G8" s="153"/>
+      <c r="H8" s="153"/>
+      <c r="I8" s="153"/>
+      <c r="J8" s="153"/>
+      <c r="K8" s="153"/>
+      <c r="L8" s="153"/>
+      <c r="M8" s="153"/>
+      <c r="N8" s="153"/>
     </row>
     <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="134" t="s">
+      <c r="A11" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="152"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
@@ -15983,7 +17196,7 @@
         <v>10</v>
       </c>
       <c r="E30" s="111">
-        <f t="shared" ref="E30:J30" si="2">SUM(E22,E14)</f>
+        <f t="shared" ref="E30:I30" si="2">SUM(E22,E14)</f>
         <v>15</v>
       </c>
       <c r="F30" s="111">
@@ -16010,12 +17223,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="G5:N5"/>
     <mergeCell ref="A6:E7"/>
     <mergeCell ref="G6:N7"/>
     <mergeCell ref="G8:K8"/>
     <mergeCell ref="L8:N8"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16069,65 +17282,65 @@
         <v>31</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="G5" s="137" t="s">
+      <c r="G5" s="154" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="137"/>
-      <c r="I5" s="137"/>
-      <c r="J5" s="137"/>
-      <c r="K5" s="137"/>
-      <c r="L5" s="137"/>
-      <c r="M5" s="137"/>
-      <c r="N5" s="137"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="154"/>
+      <c r="L5" s="154"/>
+      <c r="M5" s="154"/>
+      <c r="N5" s="154"/>
     </row>
     <row r="6" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="136" t="s">
+      <c r="A6" s="153" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="136"/>
-      <c r="M6" s="136"/>
-      <c r="N6" s="136"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="153"/>
+      <c r="G6" s="153"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="153"/>
+      <c r="M6" s="153"/>
+      <c r="N6" s="153"/>
     </row>
     <row r="7" spans="1:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="136"/>
-      <c r="B7" s="136"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="136"/>
-      <c r="I7" s="136"/>
-      <c r="J7" s="136"/>
-      <c r="K7" s="136"/>
-      <c r="L7" s="136"/>
-      <c r="M7" s="136"/>
-      <c r="N7" s="136"/>
+      <c r="A7" s="153"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="153"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="153"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
+      <c r="L7" s="153"/>
+      <c r="M7" s="153"/>
+      <c r="N7" s="153"/>
     </row>
     <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="136"/>
-      <c r="L8" s="136"/>
-      <c r="M8" s="136"/>
-      <c r="N8" s="136"/>
+      <c r="G8" s="153"/>
+      <c r="H8" s="153"/>
+      <c r="I8" s="153"/>
+      <c r="J8" s="153"/>
+      <c r="K8" s="153"/>
+      <c r="L8" s="153"/>
+      <c r="M8" s="153"/>
+      <c r="N8" s="153"/>
     </row>
     <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="134" t="s">
+      <c r="A11" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="152"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
@@ -16876,11 +18089,11 @@
       <c r="P29" s="90"/>
     </row>
     <row r="30" spans="1:16" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="138"/>
+      <c r="A30" s="136"/>
       <c r="B30" s="93" t="s">
         <v>149</v>
       </c>
-      <c r="C30" s="147">
+      <c r="C30" s="145">
         <v>5</v>
       </c>
       <c r="D30" s="34">
@@ -16904,7 +18117,7 @@
       <c r="J30" s="34">
         <v>5</v>
       </c>
-      <c r="K30" s="150" t="s">
+      <c r="K30" s="148" t="s">
         <v>48</v>
       </c>
       <c r="M30" s="113"/>
@@ -16913,11 +18126,11 @@
       <c r="P30" s="90"/>
     </row>
     <row r="31" spans="1:16" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="138"/>
+      <c r="A31" s="136"/>
       <c r="B31" s="93" t="s">
         <v>150</v>
       </c>
-      <c r="C31" s="147">
+      <c r="C31" s="145">
         <v>5</v>
       </c>
       <c r="D31" s="34">
@@ -16941,7 +18154,7 @@
       <c r="J31" s="34">
         <v>5</v>
       </c>
-      <c r="K31" s="150" t="s">
+      <c r="K31" s="148" t="s">
         <v>48</v>
       </c>
       <c r="M31" s="113"/>
@@ -16949,9 +18162,9 @@
       <c r="O31" s="90"/>
       <c r="P31" s="90"/>
     </row>
-    <row r="32" spans="1:16" s="140" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="138" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="123"/>
-      <c r="B32" s="139"/>
+      <c r="B32" s="137"/>
       <c r="C32" s="117"/>
       <c r="D32" s="118"/>
       <c r="E32" s="118"/>
@@ -16960,7 +18173,7 @@
       <c r="H32" s="118"/>
       <c r="I32" s="118"/>
       <c r="J32" s="118"/>
-      <c r="K32" s="143"/>
+      <c r="K32" s="141"/>
       <c r="M32" s="113"/>
       <c r="N32" s="90"/>
       <c r="O32" s="90"/>
@@ -16970,48 +18183,48 @@
       <c r="B33" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="141">
+      <c r="C33" s="139">
         <f>SUM(C22,C14)</f>
         <v>75</v>
       </c>
-      <c r="D33" s="141">
+      <c r="D33" s="139">
         <f>SUM(D22,D14)</f>
         <v>5</v>
       </c>
-      <c r="E33" s="141">
+      <c r="E33" s="139">
         <f t="shared" ref="E33:I33" si="2">SUM(E22,E14)</f>
         <v>10</v>
       </c>
-      <c r="F33" s="141">
+      <c r="F33" s="139">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="G33" s="141">
+      <c r="G33" s="139">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="H33" s="141">
+      <c r="H33" s="139">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="I33" s="141">
+      <c r="I33" s="139">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J33" s="141">
+      <c r="J33" s="139">
         <f>SUM(J22,J14)</f>
         <v>10</v>
       </c>
-      <c r="K33" s="142"/>
+      <c r="K33" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="G5:N5"/>
     <mergeCell ref="A6:E7"/>
     <mergeCell ref="G6:N7"/>
     <mergeCell ref="G8:K8"/>
     <mergeCell ref="L8:N8"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17023,10 +18236,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q50" sqref="Q50"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17065,65 +18278,65 @@
         <v>31</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="G5" s="137" t="s">
+      <c r="G5" s="154" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="137"/>
-      <c r="I5" s="137"/>
-      <c r="J5" s="137"/>
-      <c r="K5" s="137"/>
-      <c r="L5" s="137"/>
-      <c r="M5" s="137"/>
-      <c r="N5" s="137"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="154"/>
+      <c r="L5" s="154"/>
+      <c r="M5" s="154"/>
+      <c r="N5" s="154"/>
     </row>
     <row r="6" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="136" t="s">
+      <c r="A6" s="153" t="s">
         <v>160</v>
       </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="136"/>
-      <c r="M6" s="136"/>
-      <c r="N6" s="136"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="153"/>
+      <c r="G6" s="153"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="153"/>
+      <c r="M6" s="153"/>
+      <c r="N6" s="153"/>
     </row>
     <row r="7" spans="1:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="136"/>
-      <c r="B7" s="136"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="136"/>
-      <c r="I7" s="136"/>
-      <c r="J7" s="136"/>
-      <c r="K7" s="136"/>
-      <c r="L7" s="136"/>
-      <c r="M7" s="136"/>
-      <c r="N7" s="136"/>
+      <c r="A7" s="153"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="153"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="153"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
+      <c r="L7" s="153"/>
+      <c r="M7" s="153"/>
+      <c r="N7" s="153"/>
     </row>
     <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="136"/>
-      <c r="L8" s="136"/>
-      <c r="M8" s="136"/>
-      <c r="N8" s="136"/>
+      <c r="G8" s="153"/>
+      <c r="H8" s="153"/>
+      <c r="I8" s="153"/>
+      <c r="J8" s="153"/>
+      <c r="K8" s="153"/>
+      <c r="L8" s="153"/>
+      <c r="M8" s="153"/>
+      <c r="N8" s="153"/>
     </row>
     <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="134" t="s">
+      <c r="A11" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="152"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
@@ -17210,15 +18423,15 @@
         <v>29</v>
       </c>
       <c r="N13" s="98">
-        <f>D44</f>
+        <f>D39</f>
         <v>20</v>
       </c>
       <c r="O13" s="100">
-        <f>C44 - N13</f>
+        <f>C39 - N13</f>
         <v>100</v>
       </c>
       <c r="P13" s="99">
-        <f>C44 - N22</f>
+        <f>C39 - N22</f>
         <v>102.85714285714286</v>
       </c>
     </row>
@@ -17265,7 +18478,7 @@
         <v>30</v>
       </c>
       <c r="N14" s="98">
-        <f>E44</f>
+        <f>E39</f>
         <v>27</v>
       </c>
       <c r="O14" s="100">
@@ -17313,7 +18526,7 @@
         <v>32</v>
       </c>
       <c r="N15" s="98">
-        <f>F44</f>
+        <f>F39</f>
         <v>31</v>
       </c>
       <c r="O15" s="100">
@@ -17361,7 +18574,7 @@
         <v>33</v>
       </c>
       <c r="N16" s="98">
-        <f>G44</f>
+        <f>G39</f>
         <v>8</v>
       </c>
       <c r="O16" s="100">
@@ -17375,41 +18588,41 @@
     </row>
     <row r="17" spans="1:16" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A17" s="31"/>
-      <c r="B17" s="151" t="s">
+      <c r="B17" s="149" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="144">
+      <c r="C17" s="142">
         <v>5</v>
       </c>
-      <c r="D17" s="145">
-        <v>0</v>
-      </c>
-      <c r="E17" s="145">
+      <c r="D17" s="143">
+        <v>0</v>
+      </c>
+      <c r="E17" s="143">
         <v>5</v>
       </c>
-      <c r="F17" s="145">
-        <v>0</v>
-      </c>
-      <c r="G17" s="145">
-        <v>0</v>
-      </c>
-      <c r="H17" s="145">
-        <v>0</v>
-      </c>
-      <c r="I17" s="145">
-        <v>0</v>
-      </c>
-      <c r="J17" s="145">
-        <v>0</v>
-      </c>
-      <c r="K17" s="146" t="s">
+      <c r="F17" s="143">
+        <v>0</v>
+      </c>
+      <c r="G17" s="143">
+        <v>0</v>
+      </c>
+      <c r="H17" s="143">
+        <v>0</v>
+      </c>
+      <c r="I17" s="143">
+        <v>0</v>
+      </c>
+      <c r="J17" s="143">
+        <v>0</v>
+      </c>
+      <c r="K17" s="144" t="s">
         <v>48</v>
       </c>
       <c r="M17" s="12" t="s">
         <v>34</v>
       </c>
       <c r="N17" s="98">
-        <f>H44</f>
+        <f>H39</f>
         <v>25</v>
       </c>
       <c r="O17" s="100">
@@ -17437,7 +18650,7 @@
         <v>35</v>
       </c>
       <c r="N18" s="98">
-        <f>I44</f>
+        <f>I39</f>
         <v>0</v>
       </c>
       <c r="O18" s="100">
@@ -17450,7 +18663,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="152">
+      <c r="A19" s="150">
         <v>14</v>
       </c>
       <c r="B19" s="74" t="s">
@@ -17460,31 +18673,31 @@
         <v>40</v>
       </c>
       <c r="D19" s="128">
-        <f>SUM(D20:D25)</f>
+        <f t="shared" ref="D19:J19" si="1">SUM(D20:D25)</f>
         <v>0</v>
       </c>
       <c r="E19" s="128">
-        <f>SUM(E20:E25)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F19" s="128">
-        <f>SUM(F20:F25)</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="G19" s="128">
-        <f>SUM(G20:G25)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H19" s="128">
-        <f>SUM(H20:H25)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I19" s="128">
-        <f>SUM(I20:I25)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J19" s="128">
-        <f>SUM(J20:J25)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K19" s="129"/>
@@ -17492,7 +18705,7 @@
         <v>36</v>
       </c>
       <c r="N19" s="98">
-        <f>J44</f>
+        <f>J39</f>
         <v>14</v>
       </c>
       <c r="O19" s="100">
@@ -17608,7 +18821,7 @@
         <v>84</v>
       </c>
       <c r="N22" s="104">
-        <f xml:space="preserve"> C44 / 7</f>
+        <f xml:space="preserve"> C39 / 7</f>
         <v>17.142857142857142</v>
       </c>
     </row>
@@ -17744,27 +18957,27 @@
         <v>0</v>
       </c>
       <c r="E27" s="128">
-        <f t="shared" ref="E27:J27" si="1">SUM(E28:E37)</f>
+        <f t="shared" ref="E27:J27" si="2">SUM(E28:E37)</f>
         <v>0</v>
       </c>
       <c r="F27" s="128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G27" s="128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H27" s="128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="I27" s="128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J27" s="128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="K27" s="129"/>
@@ -17810,7 +19023,7 @@
       <c r="O28" s="90"/>
       <c r="P28" s="90"/>
     </row>
-    <row r="29" spans="1:16" s="140" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="138" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="31"/>
       <c r="B29" s="60" t="s">
         <v>171</v>
@@ -18013,7 +19226,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="138"/>
+      <c r="A35" s="136"/>
       <c r="B35" s="93" t="s">
         <v>177</v>
       </c>
@@ -18041,10 +19254,10 @@
       <c r="J35" s="34">
         <v>5</v>
       </c>
-      <c r="K35" s="146"/>
+      <c r="K35" s="144"/>
     </row>
     <row r="36" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="138"/>
+      <c r="A36" s="136"/>
       <c r="B36" s="93" t="s">
         <v>178</v>
       </c>
@@ -18072,10 +19285,10 @@
       <c r="J36" s="34">
         <v>2</v>
       </c>
-      <c r="K36" s="146"/>
+      <c r="K36" s="144"/>
     </row>
     <row r="37" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="138"/>
+      <c r="A37" s="136"/>
       <c r="B37" s="93" t="s">
         <v>179</v>
       </c>
@@ -18103,54 +19316,1140 @@
       <c r="J37" s="34">
         <v>2</v>
       </c>
-      <c r="K37" s="146"/>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="43" t="s">
+      <c r="K37" s="144"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="141">
-        <f>SUM(C19,C14,C27)</f>
+      <c r="C39" s="139">
+        <f t="shared" ref="C39:J39" si="3">SUM(C19,C14,C27)</f>
         <v>120</v>
       </c>
-      <c r="D44" s="141">
-        <f t="shared" ref="D44:J44" si="2">SUM(D19,D14,D27)</f>
+      <c r="D39" s="139">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="E44" s="141">
-        <f t="shared" si="2"/>
+      <c r="E39" s="139">
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="F44" s="141">
-        <f t="shared" si="2"/>
+      <c r="F39" s="139">
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="G44" s="141">
-        <f t="shared" si="2"/>
+      <c r="G39" s="139">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="H44" s="141">
-        <f t="shared" si="2"/>
+      <c r="H39" s="139">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="I44" s="141">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J44" s="141">
-        <f>SUM(J19,J14,J27)</f>
+      <c r="I39" s="139">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="139">
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="K44" s="142"/>
+      <c r="K39" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="G5:N5"/>
     <mergeCell ref="A6:E7"/>
     <mergeCell ref="G6:N7"/>
     <mergeCell ref="G8:K8"/>
     <mergeCell ref="L8:N8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31D3346-4EF3-42A5-A710-5BB889533B76}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:P44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:J37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" style="135" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" style="135" customWidth="1"/>
+    <col min="3" max="6" width="14.42578125" style="135"/>
+    <col min="7" max="7" width="16.140625" style="135" customWidth="1"/>
+    <col min="8" max="10" width="14.42578125" style="135"/>
+    <col min="11" max="11" width="19.5703125" style="135" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" style="135" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" style="135" customWidth="1"/>
+    <col min="14" max="14" width="16" style="135" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="135" customWidth="1"/>
+    <col min="16" max="16" width="27.28515625" style="135" customWidth="1"/>
+    <col min="17" max="16384" width="14.42578125" style="135"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="134" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="G5" s="154" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="154"/>
+      <c r="L5" s="154"/>
+      <c r="M5" s="154"/>
+      <c r="N5" s="154"/>
+    </row>
+    <row r="6" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="153"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="153"/>
+      <c r="G6" s="153"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="153"/>
+      <c r="M6" s="153"/>
+      <c r="N6" s="153"/>
+    </row>
+    <row r="7" spans="1:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="153"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="153"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="153"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
+      <c r="L7" s="153"/>
+      <c r="M7" s="153"/>
+      <c r="N7" s="153"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="G8" s="153"/>
+      <c r="H8" s="153"/>
+      <c r="I8" s="153"/>
+      <c r="J8" s="153"/>
+      <c r="K8" s="153"/>
+      <c r="L8" s="153"/>
+      <c r="M8" s="153"/>
+      <c r="N8" s="153"/>
+    </row>
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="151" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="152"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="21"/>
+      <c r="M12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="106" t="s">
+        <v>85</v>
+      </c>
+      <c r="O12" s="107" t="s">
+        <v>86</v>
+      </c>
+      <c r="P12" s="106" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="91">
+        <v>43892</v>
+      </c>
+      <c r="E13" s="91">
+        <v>43893</v>
+      </c>
+      <c r="F13" s="91">
+        <v>43894</v>
+      </c>
+      <c r="G13" s="91">
+        <v>43895</v>
+      </c>
+      <c r="H13" s="91">
+        <v>43896</v>
+      </c>
+      <c r="I13" s="91">
+        <v>43897</v>
+      </c>
+      <c r="J13" s="91">
+        <v>43898</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="98">
+        <f>D44</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="100">
+        <f>C44 - N13</f>
+        <v>120</v>
+      </c>
+      <c r="P13" s="99">
+        <f>C44 - N22</f>
+        <v>102.85714285714286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="87">
+        <v>13</v>
+      </c>
+      <c r="B14" s="57"/>
+      <c r="C14" s="88">
+        <v>40</v>
+      </c>
+      <c r="D14" s="89">
+        <v>0</v>
+      </c>
+      <c r="E14" s="89">
+        <v>0</v>
+      </c>
+      <c r="F14" s="89">
+        <v>0</v>
+      </c>
+      <c r="G14" s="89">
+        <v>0</v>
+      </c>
+      <c r="H14" s="89">
+        <v>0</v>
+      </c>
+      <c r="I14" s="89">
+        <v>0</v>
+      </c>
+      <c r="J14" s="89">
+        <v>0</v>
+      </c>
+      <c r="K14" s="30"/>
+      <c r="M14" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" s="98">
+        <f>E44</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="100">
+        <f>O13- N14</f>
+        <v>120</v>
+      </c>
+      <c r="P14" s="99">
+        <f>P13 - N22</f>
+        <v>85.714285714285722</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="31"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="33">
+        <v>30</v>
+      </c>
+      <c r="D15" s="34">
+        <v>0</v>
+      </c>
+      <c r="E15" s="34">
+        <v>0</v>
+      </c>
+      <c r="F15" s="34">
+        <v>0</v>
+      </c>
+      <c r="G15" s="34">
+        <v>0</v>
+      </c>
+      <c r="H15" s="34">
+        <v>0</v>
+      </c>
+      <c r="I15" s="34">
+        <v>0</v>
+      </c>
+      <c r="J15" s="34">
+        <v>0</v>
+      </c>
+      <c r="K15" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" s="98">
+        <f>F44</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="100">
+        <f>O14- N15</f>
+        <v>120</v>
+      </c>
+      <c r="P15" s="99">
+        <f>P14 - N22</f>
+        <v>68.571428571428584</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="31"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="33">
+        <v>5</v>
+      </c>
+      <c r="D16" s="34">
+        <v>0</v>
+      </c>
+      <c r="E16" s="34">
+        <v>0</v>
+      </c>
+      <c r="F16" s="34">
+        <v>0</v>
+      </c>
+      <c r="G16" s="34">
+        <v>0</v>
+      </c>
+      <c r="H16" s="34">
+        <v>0</v>
+      </c>
+      <c r="I16" s="34">
+        <v>0</v>
+      </c>
+      <c r="J16" s="34">
+        <v>0</v>
+      </c>
+      <c r="K16" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" s="98">
+        <f>G44</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="100">
+        <f>O15- N16</f>
+        <v>120</v>
+      </c>
+      <c r="P16" s="99">
+        <f>P15 - N22</f>
+        <v>51.428571428571445</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="31"/>
+      <c r="B17" s="149"/>
+      <c r="C17" s="142">
+        <v>5</v>
+      </c>
+      <c r="D17" s="34">
+        <v>0</v>
+      </c>
+      <c r="E17" s="34">
+        <v>0</v>
+      </c>
+      <c r="F17" s="34">
+        <v>0</v>
+      </c>
+      <c r="G17" s="34">
+        <v>0</v>
+      </c>
+      <c r="H17" s="34">
+        <v>0</v>
+      </c>
+      <c r="I17" s="34">
+        <v>0</v>
+      </c>
+      <c r="J17" s="34">
+        <v>0</v>
+      </c>
+      <c r="K17" s="144" t="s">
+        <v>48</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" s="98">
+        <f>H44</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="100">
+        <f>O16- N17</f>
+        <v>120</v>
+      </c>
+      <c r="P17" s="99">
+        <f>P16 - N22</f>
+        <v>34.285714285714306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="40"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="117"/>
+      <c r="M18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N18" s="98">
+        <f>I44</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="100">
+        <f>O17- N18</f>
+        <v>120</v>
+      </c>
+      <c r="P18" s="99">
+        <f>P17 - N22</f>
+        <v>17.142857142857164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="150">
+        <v>14</v>
+      </c>
+      <c r="B19" s="74"/>
+      <c r="C19" s="127">
+        <v>40</v>
+      </c>
+      <c r="D19" s="128">
+        <f t="shared" ref="D19:J19" si="0">SUM(D20:D25)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="128">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="128">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="128">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="128">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="128">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="128">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="129"/>
+      <c r="M19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N19" s="98">
+        <f>J44</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="100">
+        <v>0</v>
+      </c>
+      <c r="P19" s="99">
+        <f>P18 - N22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="31"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="126">
+        <v>2</v>
+      </c>
+      <c r="D20" s="34">
+        <v>0</v>
+      </c>
+      <c r="E20" s="34">
+        <v>0</v>
+      </c>
+      <c r="F20" s="34">
+        <v>0</v>
+      </c>
+      <c r="G20" s="34">
+        <v>0</v>
+      </c>
+      <c r="H20" s="34">
+        <v>0</v>
+      </c>
+      <c r="I20" s="34">
+        <v>0</v>
+      </c>
+      <c r="J20" s="34">
+        <v>0</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="90" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="31"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="126">
+        <v>5</v>
+      </c>
+      <c r="D21" s="34">
+        <v>0</v>
+      </c>
+      <c r="E21" s="34">
+        <v>0</v>
+      </c>
+      <c r="F21" s="34">
+        <v>0</v>
+      </c>
+      <c r="G21" s="34">
+        <v>0</v>
+      </c>
+      <c r="H21" s="34">
+        <v>0</v>
+      </c>
+      <c r="I21" s="34">
+        <v>0</v>
+      </c>
+      <c r="J21" s="34">
+        <v>0</v>
+      </c>
+      <c r="K21" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M21" s="113"/>
+      <c r="O21" s="135"/>
+      <c r="P21" s="135"/>
+    </row>
+    <row r="22" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="31"/>
+      <c r="B22" s="130"/>
+      <c r="C22" s="126">
+        <v>15</v>
+      </c>
+      <c r="D22" s="34">
+        <v>0</v>
+      </c>
+      <c r="E22" s="34">
+        <v>0</v>
+      </c>
+      <c r="F22" s="34">
+        <v>0</v>
+      </c>
+      <c r="G22" s="34">
+        <v>0</v>
+      </c>
+      <c r="H22" s="34">
+        <v>0</v>
+      </c>
+      <c r="I22" s="34">
+        <v>0</v>
+      </c>
+      <c r="J22" s="34">
+        <v>0</v>
+      </c>
+      <c r="K22" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M22" s="103" t="s">
+        <v>84</v>
+      </c>
+      <c r="N22" s="104">
+        <f xml:space="preserve"> C44 / 7</f>
+        <v>17.142857142857142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="40"/>
+      <c r="B23" s="130"/>
+      <c r="C23" s="126">
+        <v>8</v>
+      </c>
+      <c r="D23" s="34">
+        <v>0</v>
+      </c>
+      <c r="E23" s="34">
+        <v>0</v>
+      </c>
+      <c r="F23" s="34">
+        <v>0</v>
+      </c>
+      <c r="G23" s="34">
+        <v>0</v>
+      </c>
+      <c r="H23" s="34">
+        <v>0</v>
+      </c>
+      <c r="I23" s="34">
+        <v>0</v>
+      </c>
+      <c r="J23" s="34">
+        <v>0</v>
+      </c>
+      <c r="K23" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="123"/>
+      <c r="N23" s="123"/>
+      <c r="O23" s="124"/>
+      <c r="P23" s="123"/>
+    </row>
+    <row r="24" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="40"/>
+      <c r="B24" s="130"/>
+      <c r="C24" s="126">
+        <v>8</v>
+      </c>
+      <c r="D24" s="34">
+        <v>0</v>
+      </c>
+      <c r="E24" s="34">
+        <v>0</v>
+      </c>
+      <c r="F24" s="34">
+        <v>0</v>
+      </c>
+      <c r="G24" s="34">
+        <v>0</v>
+      </c>
+      <c r="H24" s="34">
+        <v>0</v>
+      </c>
+      <c r="I24" s="34">
+        <v>0</v>
+      </c>
+      <c r="J24" s="34">
+        <v>0</v>
+      </c>
+      <c r="K24" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M24" s="123"/>
+      <c r="N24" s="123"/>
+      <c r="O24" s="124"/>
+      <c r="P24" s="123"/>
+    </row>
+    <row r="25" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="40"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="126">
+        <v>7</v>
+      </c>
+      <c r="D25" s="34">
+        <v>0</v>
+      </c>
+      <c r="E25" s="34">
+        <v>0</v>
+      </c>
+      <c r="F25" s="34">
+        <v>0</v>
+      </c>
+      <c r="G25" s="34">
+        <v>0</v>
+      </c>
+      <c r="H25" s="34">
+        <v>0</v>
+      </c>
+      <c r="I25" s="34">
+        <v>0</v>
+      </c>
+      <c r="J25" s="34">
+        <v>0</v>
+      </c>
+      <c r="K25" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M25" s="123"/>
+      <c r="N25" s="123"/>
+      <c r="O25" s="124"/>
+      <c r="P25" s="123"/>
+    </row>
+    <row r="26" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="M26" s="113"/>
+      <c r="N26" s="90"/>
+      <c r="O26" s="90"/>
+      <c r="P26" s="90"/>
+    </row>
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="125">
+        <v>15</v>
+      </c>
+      <c r="B27" s="74"/>
+      <c r="C27" s="127">
+        <v>40</v>
+      </c>
+      <c r="D27" s="128">
+        <f>SUM(D28:D37)</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="128">
+        <f t="shared" ref="E27:J27" si="1">SUM(E28:E37)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="128">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="128">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="128">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="128">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="128">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="129"/>
+      <c r="M27" s="113"/>
+      <c r="N27" s="90"/>
+      <c r="O27" s="90"/>
+      <c r="P27" s="90"/>
+    </row>
+    <row r="28" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="31"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="126">
+        <v>1</v>
+      </c>
+      <c r="D28" s="34">
+        <v>0</v>
+      </c>
+      <c r="E28" s="34">
+        <v>0</v>
+      </c>
+      <c r="F28" s="34">
+        <v>0</v>
+      </c>
+      <c r="G28" s="34">
+        <v>0</v>
+      </c>
+      <c r="H28" s="34">
+        <v>0</v>
+      </c>
+      <c r="I28" s="34">
+        <v>0</v>
+      </c>
+      <c r="J28" s="34">
+        <v>0</v>
+      </c>
+      <c r="K28" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M28" s="113"/>
+      <c r="N28" s="90"/>
+      <c r="O28" s="90"/>
+      <c r="P28" s="90"/>
+    </row>
+    <row r="29" spans="1:16" s="138" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="31"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="126">
+        <v>5</v>
+      </c>
+      <c r="D29" s="34">
+        <v>0</v>
+      </c>
+      <c r="E29" s="34">
+        <v>0</v>
+      </c>
+      <c r="F29" s="34">
+        <v>0</v>
+      </c>
+      <c r="G29" s="34">
+        <v>0</v>
+      </c>
+      <c r="H29" s="34">
+        <v>0</v>
+      </c>
+      <c r="I29" s="34">
+        <v>0</v>
+      </c>
+      <c r="J29" s="34">
+        <v>0</v>
+      </c>
+      <c r="K29" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M29" s="113"/>
+      <c r="N29" s="90"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="90"/>
+    </row>
+    <row r="30" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="31"/>
+      <c r="B30" s="130"/>
+      <c r="C30" s="126">
+        <v>5</v>
+      </c>
+      <c r="D30" s="34">
+        <v>0</v>
+      </c>
+      <c r="E30" s="34">
+        <v>0</v>
+      </c>
+      <c r="F30" s="34">
+        <v>0</v>
+      </c>
+      <c r="G30" s="34">
+        <v>0</v>
+      </c>
+      <c r="H30" s="34">
+        <v>0</v>
+      </c>
+      <c r="I30" s="34">
+        <v>0</v>
+      </c>
+      <c r="J30" s="34">
+        <v>0</v>
+      </c>
+      <c r="K30" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="40"/>
+      <c r="B31" s="130"/>
+      <c r="C31" s="126">
+        <v>5</v>
+      </c>
+      <c r="D31" s="34">
+        <v>0</v>
+      </c>
+      <c r="E31" s="34">
+        <v>0</v>
+      </c>
+      <c r="F31" s="34">
+        <v>0</v>
+      </c>
+      <c r="G31" s="34">
+        <v>0</v>
+      </c>
+      <c r="H31" s="34">
+        <v>0</v>
+      </c>
+      <c r="I31" s="34">
+        <v>0</v>
+      </c>
+      <c r="J31" s="34">
+        <v>0</v>
+      </c>
+      <c r="K31" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="40"/>
+      <c r="B32" s="131"/>
+      <c r="C32" s="126">
+        <v>5</v>
+      </c>
+      <c r="D32" s="34">
+        <v>0</v>
+      </c>
+      <c r="E32" s="34">
+        <v>0</v>
+      </c>
+      <c r="F32" s="34">
+        <v>0</v>
+      </c>
+      <c r="G32" s="34">
+        <v>0</v>
+      </c>
+      <c r="H32" s="34">
+        <v>0</v>
+      </c>
+      <c r="I32" s="34">
+        <v>0</v>
+      </c>
+      <c r="J32" s="34">
+        <v>0</v>
+      </c>
+      <c r="K32" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="40"/>
+      <c r="B33" s="132"/>
+      <c r="C33" s="126">
+        <v>5</v>
+      </c>
+      <c r="D33" s="34">
+        <v>0</v>
+      </c>
+      <c r="E33" s="34">
+        <v>0</v>
+      </c>
+      <c r="F33" s="34">
+        <v>0</v>
+      </c>
+      <c r="G33" s="34">
+        <v>0</v>
+      </c>
+      <c r="H33" s="34">
+        <v>0</v>
+      </c>
+      <c r="I33" s="34">
+        <v>0</v>
+      </c>
+      <c r="J33" s="34">
+        <v>0</v>
+      </c>
+      <c r="K33" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="40"/>
+      <c r="B34" s="132"/>
+      <c r="C34" s="126">
+        <v>5</v>
+      </c>
+      <c r="D34" s="34">
+        <v>0</v>
+      </c>
+      <c r="E34" s="34">
+        <v>0</v>
+      </c>
+      <c r="F34" s="34">
+        <v>0</v>
+      </c>
+      <c r="G34" s="34">
+        <v>0</v>
+      </c>
+      <c r="H34" s="34">
+        <v>0</v>
+      </c>
+      <c r="I34" s="34">
+        <v>0</v>
+      </c>
+      <c r="J34" s="34">
+        <v>0</v>
+      </c>
+      <c r="K34" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="136"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="126">
+        <v>5</v>
+      </c>
+      <c r="D35" s="34">
+        <v>0</v>
+      </c>
+      <c r="E35" s="34">
+        <v>0</v>
+      </c>
+      <c r="F35" s="34">
+        <v>0</v>
+      </c>
+      <c r="G35" s="34">
+        <v>0</v>
+      </c>
+      <c r="H35" s="34">
+        <v>0</v>
+      </c>
+      <c r="I35" s="34">
+        <v>0</v>
+      </c>
+      <c r="J35" s="34">
+        <v>0</v>
+      </c>
+      <c r="K35" s="144"/>
+    </row>
+    <row r="36" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="136"/>
+      <c r="B36" s="93"/>
+      <c r="C36" s="126">
+        <v>2</v>
+      </c>
+      <c r="D36" s="34">
+        <v>0</v>
+      </c>
+      <c r="E36" s="34">
+        <v>0</v>
+      </c>
+      <c r="F36" s="34">
+        <v>0</v>
+      </c>
+      <c r="G36" s="34">
+        <v>0</v>
+      </c>
+      <c r="H36" s="34">
+        <v>0</v>
+      </c>
+      <c r="I36" s="34">
+        <v>0</v>
+      </c>
+      <c r="J36" s="34">
+        <v>0</v>
+      </c>
+      <c r="K36" s="144"/>
+    </row>
+    <row r="37" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="136"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="126">
+        <v>2</v>
+      </c>
+      <c r="D37" s="34">
+        <v>0</v>
+      </c>
+      <c r="E37" s="34">
+        <v>0</v>
+      </c>
+      <c r="F37" s="34">
+        <v>0</v>
+      </c>
+      <c r="G37" s="34">
+        <v>0</v>
+      </c>
+      <c r="H37" s="34">
+        <v>0</v>
+      </c>
+      <c r="I37" s="34">
+        <v>0</v>
+      </c>
+      <c r="J37" s="34">
+        <v>0</v>
+      </c>
+      <c r="K37" s="144"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="139">
+        <f>SUM(C19,C14,C27)</f>
+        <v>120</v>
+      </c>
+      <c r="D44" s="139">
+        <f t="shared" ref="D44:I44" si="2">SUM(D19,D14,D27)</f>
+        <v>0</v>
+      </c>
+      <c r="E44" s="139">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="139">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G44" s="139">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="139">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="139">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="139">
+        <f>SUM(J19,J14,J27)</f>
+        <v>0</v>
+      </c>
+      <c r="K44" s="140"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="A6:E7"/>
+    <mergeCell ref="G6:N7"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="L8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added unit tests to test statists classes, outliers and other functions
</commit_message>
<xml_diff>
--- a/Documentation/Q5031372-ArtifactDiary/Product & Sprint Backlog.xlsx
+++ b/Documentation/Q5031372-ArtifactDiary/Product & Sprint Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Year Three\ComputingProject\ShellTemperature\Documentation\Q5031372-ArtifactDiary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003F7407-C5E8-4464-83C8-5EE207F07BD2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DE0CFB-4C11-4560-977C-F86D63997F97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46305" yWindow="6360" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="181">
   <si>
     <t>UserStoryID</t>
   </si>
@@ -16374,7 +16374,7 @@
   </sheetPr>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -17242,7 +17242,7 @@
   </sheetPr>
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
@@ -18238,8 +18238,8 @@
   </sheetPr>
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:K39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -19254,7 +19254,9 @@
       <c r="J35" s="34">
         <v>5</v>
       </c>
-      <c r="K35" s="144"/>
+      <c r="K35" s="144" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="136"/>
@@ -19285,7 +19287,9 @@
       <c r="J36" s="34">
         <v>2</v>
       </c>
-      <c r="K36" s="144"/>
+      <c r="K36" s="144" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="136"/>
@@ -19316,7 +19320,9 @@
       <c r="J37" s="34">
         <v>2</v>
       </c>
-      <c r="K37" s="144"/>
+      <c r="K37" s="144" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="43" t="s">

</xml_diff>